<commit_message>
Exercícios bloco 9 feitos
</commit_message>
<xml_diff>
--- a/bloco9/9_3/História da Vida.xlsx
+++ b/bloco9/9_3/História da Vida.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rfrei\t_git\bloco9\9_3\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19185" windowHeight="5085"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Página1" sheetId="1" r:id="rId4"/>
+    <sheet name="Página1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>História da Vida</t>
   </si>
@@ -47,27 +55,68 @@
   </si>
   <si>
     <t>Escolhas significativas</t>
+  </si>
+  <si>
+    <t>21 a 28 anos</t>
+  </si>
+  <si>
+    <t>Minha irmã nasceu</t>
+  </si>
+  <si>
+    <t>Minha vó faleceu</t>
+  </si>
+  <si>
+    <t>Amizades? Tinha um pessoal barra pesada no meu bairro</t>
+  </si>
+  <si>
+    <t>Vários, foi a melhor época. O mais marcante foi ter escolhido viver em república durante a faculdade. Conheci minha atual namorada/futura esposa</t>
+  </si>
+  <si>
+    <t>O curso que escolhi, as pessoas que decidi seguir sendo próximo. Concorrer a bolsa de estudos do ciências sem fronteiras.</t>
+  </si>
+  <si>
+    <t>Vários também, neste período fui para o intercâmbio, finalizei a faculdade, comecei meu primeiro emprego, empreendi em um novo ramo, abandonei tudo e recomecei</t>
+  </si>
+  <si>
+    <t>Meus pais se separaram, e tive um afastamento novamente de amigos, por conta de trabalho e estudos.</t>
+  </si>
+  <si>
+    <t>Iniciar/abandonar empregos, empreendimentos. Perdoar algumas pessoas, me afastar de outras.</t>
+  </si>
+  <si>
+    <t>Mudei para uma escola melhor, com uma estrutura muito legal, além de mudar de bairro, para uma casa melhor.</t>
+  </si>
+  <si>
+    <t>Mais uma vez me afastei de muitos amigos, pela mudança. Me separei da minha primeira namorada.</t>
+  </si>
+  <si>
+    <t>Perdi meus amigos pela mudança, fiquei um pouco isolado devido ao bairro ter mt menos crianças.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concorrer à bolsa escolar e ser premiado, pois meus pais precisaram disso. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color rgb="FF34A853"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -75,7 +124,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -85,41 +134,53 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" textRotation="90" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -309,30 +370,45 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="4.86"/>
-    <col customWidth="1" min="2" max="9" width="20.0"/>
+    <col min="1" max="1" width="4.85546875" style="5" customWidth="1"/>
+    <col min="2" max="10" width="20" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="14.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
     </row>
-    <row r="2">
-      <c r="A2" s="2"/>
+    <row r="2" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
@@ -343,40 +419,79 @@
         <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" ht="97.5" customHeight="1">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:10" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="4" ht="97.5" customHeight="1">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:10" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="5" ht="97.5" customHeight="1">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:10" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>